<commit_message>
Updates to summary code
</commit_message>
<xml_diff>
--- a/Summer 2015 Tree Traits.xlsx
+++ b/Summer 2015 Tree Traits.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26519"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26819"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="500" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="17460" tabRatio="500" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Metadata" sheetId="2" r:id="rId1"/>
@@ -17,7 +17,7 @@
   </definedNames>
   <calcPr calcId="140001" concurrentCalc="0"/>
   <pivotCaches>
-    <pivotCache cacheId="0" r:id="rId5"/>
+    <pivotCache cacheId="4" r:id="rId5"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
@@ -3559,7 +3559,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="179">
+  <cellStyleXfs count="181">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -3739,6 +3739,8 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="45">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
@@ -3811,7 +3813,7 @@
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
-  <cellStyles count="179">
+  <cellStyles count="181">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -3900,6 +3902,7 @@
     <cellStyle name="Followed Hyperlink" xfId="174" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="176" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="178" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="180" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -3988,6 +3991,7 @@
     <cellStyle name="Hyperlink" xfId="173" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="175" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="177" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="179" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="81"/>
     <cellStyle name="Normal 3" xfId="108"/>
@@ -7355,7 +7359,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable1" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="4" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="4" indent="0" outline="1" outlineData="1" gridDropZones="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable1" cacheId="4" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="4" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="4" indent="0" outline="1" outlineData="1" gridDropZones="1" multipleFieldFilters="0">
   <location ref="A3:F48" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
   <pivotFields count="2">
     <pivotField axis="axisCol" showAll="0">
@@ -49051,7 +49055,7 @@
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A21" sqref="A21"/>
+      <selection pane="bottomRight" activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="12" x14ac:dyDescent="0"/>

</xml_diff>